<commit_message>
LOGI & MLCO quarter update
</commit_message>
<xml_diff>
--- a/Electronic Technology - Computer Peripherals/LOGI.xlsx
+++ b/Electronic Technology - Computer Peripherals/LOGI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\models\Electronic Technology - Computer Peripherals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64ED2314-D871-46AE-B167-5956DFEAD10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBE32EE-52B7-467F-B7C3-87E63B3D3147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="120" windowWidth="14340" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,16 +21,16 @@
     <sheet name="DoR" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Model!$B$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Model!$B$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Model!$L$2:$X$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Model!$L$3:$X$3</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Model!$L$4:$X$4</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Model!$B$19</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Model!$B$20</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Model!$L$19:$X$19</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Model!$L$20:$X$20</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Model!$L$2:$X$2</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Model!$B$19</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Model!$B$20</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Model!$L$19:$X$19</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Model!$L$20:$X$20</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Model!$L$2:$X$2</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Model!$B$3</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Model!$B$4</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Model!$L$2:$X$2</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Model!$L$3:$X$3</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Model!$L$4:$X$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1693,7 +1693,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1911,6 +1911,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2212,6 +2217,9 @@
                 <c:pt idx="10">
                   <c:v>1255.473</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>1011.487</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2345,7 +2353,7 @@
                   <c:v>-1.1380199618087672E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1</c:v>
+                  <c:v>5.3547788354475712E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>-1</c:v>
@@ -2842,7 +2850,7 @@
                   <c:v>4538.8180000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4240</c:v>
+                  <c:v>4298.4669999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2974,10 +2982,10 @@
                   <c:v>-0.17191491271552917</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-6.5836083315083394E-2</c:v>
+                  <c:v>-5.2954535740362463E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7735849056603765E-2</c:v>
+                  <c:v>2.3620746652236901E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3522,7 +3530,7 @@
                   <c:v>244.68400000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>167.61499999999987</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -3672,7 +3680,7 @@
                   <c:v>0.42153116793431644</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.43444552426279326</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4133,7 +4141,7 @@
                   <c:v>364.58400000000097</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>603.20000000000005</c:v>
+                  <c:v>612.18299999999977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4254,10 +4262,10 @@
                   <c:v>-0.43432638286582015</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.65448840322120128</c:v>
+                  <c:v>0.67912744388124047</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5092838196286511E-2</c:v>
+                  <c:v>9.0078293582152025E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4933,7 +4941,7 @@
                   <c:v>5.7909648395465294E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>7.4564477843017271E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5081,7 +5089,7 @@
                   <c:v>3.1630309851346863E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3.807265936190974E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14421,18 +14429,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.9</cx:f>
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.8</cx:f>
+        <cx:f dir="row">_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.9</cx:f>
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.7</cx:f>
+        <cx:f dir="row">_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -14476,7 +14484,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{006F4749-938E-4621-8334-C74E7B83CC40}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>EPS exp.</cx:v>
             </cx:txData>
           </cx:tx>
@@ -14496,7 +14504,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C8A70830-D21B-405F-8F13-72F0AC678416}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>EPS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -14527,18 +14535,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.2</cx:f>
+        <cx:f dir="row">_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.4</cx:f>
+        <cx:f dir="row">_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.2</cx:f>
+        <cx:f dir="row">_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.3</cx:f>
+        <cx:f dir="row">_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -14582,7 +14590,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{006F4749-938E-4621-8334-C74E7B83CC40}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>Rev. Exp.</cx:v>
             </cx:txData>
           </cx:tx>
@@ -14602,7 +14610,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C8A70830-D21B-405F-8F13-72F0AC678416}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.5</cx:f>
               <cx:v>Revenue</cx:v>
             </cx:txData>
           </cx:tx>
@@ -20324,8 +20332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20378,7 +20386,7 @@
         <v>39</v>
       </c>
       <c r="C3" s="20">
-        <v>45399</v>
+        <v>45412</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>147</v>
@@ -20407,7 +20415,7 @@
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="21">
-        <v>0.70972222222222225</v>
+        <v>0.63611111111111107</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>149</v>
@@ -20690,7 +20698,7 @@
       </c>
       <c r="C14" s="36">
         <f>C6/Model!G19</f>
-        <v>21.098143236074272</v>
+        <v>20.369665671866102</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="29"/>
@@ -20717,7 +20725,7 @@
       </c>
       <c r="C16" s="6">
         <f>Model!G19/Model!F19-1</f>
-        <v>0.65524326355517082</v>
+        <v>0.71443950173752224</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
@@ -20726,7 +20734,7 @@
       </c>
       <c r="C17" s="6">
         <f>Model!H20/Model!G19-1</f>
-        <v>4.5092838196286511E-2</v>
+        <v>9.0078293582152025E-3</v>
       </c>
       <c r="E17" s="33" t="s">
         <v>52</v>
@@ -20741,7 +20749,7 @@
       </c>
       <c r="C18" s="52">
         <f>C14/C16</f>
-        <v>32.19894718428926</v>
+        <v>28.511393368265502</v>
       </c>
       <c r="L18" s="133"/>
       <c r="M18" s="134"/>
@@ -20753,7 +20761,7 @@
       </c>
       <c r="C19" s="52">
         <f>C15/C17</f>
-        <v>447.69453568229284</v>
+        <v>2241.1411735360884</v>
       </c>
       <c r="L19" s="133"/>
       <c r="M19" s="134"/>
@@ -20765,7 +20773,7 @@
       </c>
       <c r="C20" s="6">
         <f>Model!G3/Model!F3-1</f>
-        <v>-6.5836083315083394E-2</v>
+        <v>-5.2954535740362463E-2</v>
       </c>
       <c r="L20" s="133"/>
       <c r="M20" s="134"/>
@@ -20777,7 +20785,7 @@
       </c>
       <c r="C21" s="6">
         <f>Model!H4/Model!G3-1</f>
-        <v>3.7735849056603765E-2</v>
+        <v>2.3620746652236901E-2</v>
       </c>
       <c r="L21" s="133"/>
       <c r="M21" s="134"/>
@@ -20951,10 +20959,10 @@
   <dimension ref="A1:Y68"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X21" sqref="X21"/>
+      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21102,7 +21110,8 @@
         <v>4538.8180000000002</v>
       </c>
       <c r="G3" s="15">
-        <v>4240</v>
+        <f>SUM(T3:W3)</f>
+        <v>4298.4669999999996</v>
       </c>
       <c r="H3" s="41"/>
       <c r="I3" s="41"/>
@@ -21139,7 +21148,9 @@
       <c r="V3" s="10">
         <v>1255.473</v>
       </c>
-      <c r="W3" s="15"/>
+      <c r="W3" s="15">
+        <v>1011.487</v>
+      </c>
       <c r="X3" s="10"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -21184,7 +21195,10 @@
         <f>SUM(P5:S5)</f>
         <v>2806.4290000000001</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="15">
+        <f t="shared" ref="G5:G11" si="1">SUM(T5:W5)</f>
+        <v>2509.4180000000001</v>
+      </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="L5" s="10">
@@ -21220,7 +21234,9 @@
       <c r="V5" s="10">
         <v>726.25199999999995</v>
       </c>
-      <c r="W5" s="15"/>
+      <c r="W5" s="15">
+        <v>572.05100000000004</v>
+      </c>
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
     </row>
@@ -21235,10 +21251,13 @@
         <v>14.023</v>
       </c>
       <c r="F6" s="10">
-        <f t="shared" ref="F6:F11" si="1">SUM(P6:S6)</f>
+        <f t="shared" ref="F6:F11" si="2">SUM(P6:S6)</f>
         <v>12.865</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="15">
+        <f t="shared" si="1"/>
+        <v>11.027999999999999</v>
+      </c>
       <c r="H6" s="41"/>
       <c r="I6" s="41"/>
       <c r="L6" s="10">
@@ -21274,7 +21293,9 @@
       <c r="V6" s="10">
         <v>2.4409999999999998</v>
       </c>
-      <c r="W6" s="15"/>
+      <c r="W6" s="15">
+        <v>2.4590000000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -21287,10 +21308,13 @@
         <v>1025.8990000000001</v>
       </c>
       <c r="F7" s="10">
+        <f t="shared" si="2"/>
+        <v>809.18200000000002</v>
+      </c>
+      <c r="G7" s="15">
         <f t="shared" si="1"/>
-        <v>809.18200000000002</v>
-      </c>
-      <c r="G7" s="15"/>
+        <v>730.31</v>
+      </c>
       <c r="H7" s="41"/>
       <c r="I7" s="41"/>
       <c r="L7" s="10">
@@ -21326,7 +21350,9 @@
       <c r="V7" s="10">
         <v>189.17500000000001</v>
       </c>
-      <c r="W7" s="15"/>
+      <c r="W7" s="15">
+        <v>185.59399999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -21339,10 +21365,13 @@
         <v>291.84399999999999</v>
       </c>
       <c r="F8" s="10">
+        <f t="shared" si="2"/>
+        <v>280.79599999999999</v>
+      </c>
+      <c r="G8" s="15">
         <f t="shared" si="1"/>
-        <v>280.79599999999999</v>
-      </c>
-      <c r="G8" s="15"/>
+        <v>287.24299999999999</v>
+      </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="L8" s="10">
@@ -21378,7 +21407,9 @@
       <c r="V8" s="10">
         <v>72.703999999999994</v>
       </c>
-      <c r="W8" s="15"/>
+      <c r="W8" s="15">
+        <v>75.421000000000006</v>
+      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -21391,10 +21422,13 @@
         <v>148.648</v>
       </c>
       <c r="F9" s="10">
+        <f t="shared" si="2"/>
+        <v>124.652</v>
+      </c>
+      <c r="G9" s="15">
         <f t="shared" si="1"/>
-        <v>124.652</v>
-      </c>
-      <c r="G9" s="15"/>
+        <v>155.05599999999998</v>
+      </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="L9" s="10">
@@ -21430,7 +21464,9 @@
       <c r="V9" s="10">
         <v>39.710999999999999</v>
       </c>
-      <c r="W9" s="15"/>
+      <c r="W9" s="15">
+        <v>38.51</v>
+      </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -21443,10 +21479,13 @@
         <v>22.836999999999996</v>
       </c>
       <c r="F10" s="10">
+        <f t="shared" si="2"/>
+        <v>11.843000000000002</v>
+      </c>
+      <c r="G10" s="15">
         <f t="shared" si="1"/>
-        <v>11.843000000000002</v>
-      </c>
-      <c r="G10" s="15"/>
+        <v>14.209999999999999</v>
+      </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="L10" s="10">
@@ -21483,7 +21522,10 @@
       <c r="V10" s="10">
         <v>2.2759999999999998</v>
       </c>
-      <c r="W10" s="15"/>
+      <c r="W10" s="15">
+        <f>2.655+3.526-0.25</f>
+        <v>5.9309999999999992</v>
+      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -21496,10 +21538,13 @@
         <v>-0.23399999999999999</v>
       </c>
       <c r="F11" s="10">
+        <f t="shared" si="2"/>
+        <v>34.573</v>
+      </c>
+      <c r="G11" s="15">
         <f t="shared" si="1"/>
-        <v>34.573</v>
-      </c>
-      <c r="G11" s="15"/>
+        <v>3.8660000000000005</v>
+      </c>
       <c r="H11" s="41"/>
       <c r="I11" s="41"/>
       <c r="L11" s="10">
@@ -21536,96 +21581,98 @@
       <c r="V11" s="10">
         <v>0.83899999999999997</v>
       </c>
-      <c r="W11" s="15"/>
+      <c r="W11" s="15">
+        <v>1.304</v>
+      </c>
     </row>
     <row r="12" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="11">
-        <f t="shared" ref="C12:I12" si="2">C3-SUM(C5:C11)</f>
+        <f t="shared" ref="C12:I12" si="3">C3-SUM(C5:C11)</f>
         <v>0</v>
       </c>
       <c r="D12" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E12" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>774.01199999999881</v>
       </c>
       <c r="F12" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>458.47800000000097</v>
       </c>
       <c r="G12" s="14">
-        <f t="shared" si="2"/>
-        <v>4240</v>
+        <f t="shared" si="3"/>
+        <v>587.33599999999979</v>
       </c>
       <c r="H12" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I12" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11">
-        <f t="shared" ref="L12:Y12" si="3">L3-SUM(L5:L11)</f>
+        <f t="shared" ref="L12:Y12" si="4">L3-SUM(L5:L11)</f>
         <v>203.0809999999999</v>
       </c>
       <c r="M12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>179.41100000000006</v>
       </c>
       <c r="N12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>262.75099999999998</v>
       </c>
       <c r="O12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128.76900000000001</v>
       </c>
       <c r="P12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>115.47900000000004</v>
       </c>
       <c r="Q12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>127.40100000000007</v>
       </c>
       <c r="R12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>176.75399999999991</v>
       </c>
       <c r="S12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38.844000000000051</v>
       </c>
       <c r="T12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78.4050000000002</v>
       </c>
       <c r="U12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>156.63900000000012</v>
       </c>
       <c r="V12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>222.07500000000005</v>
       </c>
       <c r="W12" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>130.21699999999987</v>
+      </c>
+      <c r="X12" s="11">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X12" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="Y12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -21636,14 +21683,17 @@
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10">
-        <f t="shared" ref="E13:E14" si="4">SUM(L13:O13)</f>
+        <f t="shared" ref="E13:E14" si="5">SUM(L13:O13)</f>
         <v>1.246</v>
       </c>
       <c r="F13" s="10">
-        <f t="shared" ref="F13:F14" si="5">SUM(P13:S13)</f>
+        <f t="shared" ref="F13:F14" si="6">SUM(P13:S13)</f>
         <v>18.331</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="15">
+        <f t="shared" ref="G13:G14" si="7">SUM(T13:W13)</f>
+        <v>50.636000000000003</v>
+      </c>
       <c r="H13" s="41"/>
       <c r="I13" s="41"/>
       <c r="L13" s="10">
@@ -21680,7 +21730,9 @@
       <c r="V13" s="10">
         <v>12.826000000000001</v>
       </c>
-      <c r="W13" s="15"/>
+      <c r="W13" s="15">
+        <v>16.128</v>
+      </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -21689,14 +21741,17 @@
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="F14" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-13.278</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="15">
+        <f t="shared" si="7"/>
+        <v>-16.335999999999999</v>
+      </c>
       <c r="H14" s="41"/>
       <c r="I14" s="41"/>
       <c r="L14" s="10">
@@ -21732,94 +21787,96 @@
       <c r="V14" s="10">
         <v>0.189</v>
       </c>
-      <c r="W14" s="15"/>
+      <c r="W14" s="15">
+        <v>-2.5489999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="11">
-        <f t="shared" ref="C15:I15" si="6">C12+SUM(C13:C14)</f>
+        <f t="shared" ref="C15:I15" si="8">C12+SUM(C13:C14)</f>
         <v>0</v>
       </c>
       <c r="D15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>775.81799999999885</v>
       </c>
       <c r="F15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>463.53100000000097</v>
       </c>
       <c r="G15" s="14">
-        <f t="shared" si="6"/>
-        <v>4240</v>
+        <f t="shared" si="8"/>
+        <v>621.63599999999974</v>
       </c>
       <c r="H15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L15" s="11">
-        <f t="shared" ref="L15:Y15" si="7">L12+SUM(L13:L14)</f>
+        <f t="shared" ref="L15:Y15" si="9">L12+SUM(L13:L14)</f>
         <v>211.83199999999991</v>
       </c>
       <c r="M15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>172.90900000000005</v>
       </c>
       <c r="N15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>259.35599999999999</v>
       </c>
       <c r="O15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>131.721</v>
       </c>
       <c r="P15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>122.55200000000004</v>
       </c>
       <c r="Q15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>105.46300000000006</v>
       </c>
       <c r="R15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>182.8249999999999</v>
       </c>
       <c r="S15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>52.691000000000052</v>
       </c>
       <c r="T15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>75.259000000000199</v>
       </c>
       <c r="U15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>167.49100000000013</v>
       </c>
       <c r="V15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>235.09000000000003</v>
       </c>
       <c r="W15" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
+        <v>143.79599999999988</v>
+      </c>
+      <c r="X15" s="11">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="X15" s="11">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="Y15" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -21837,7 +21894,10 @@
         <f>SUM(P16:S16)</f>
         <v>98.947000000000003</v>
       </c>
-      <c r="G16" s="15"/>
+      <c r="G16" s="15">
+        <f>SUM(T16:W16)</f>
+        <v>9.4529999999999994</v>
+      </c>
       <c r="H16" s="41"/>
       <c r="I16" s="41"/>
       <c r="L16" s="10">
@@ -21873,7 +21933,9 @@
       <c r="V16" s="10">
         <v>-9.5939999999999994</v>
       </c>
-      <c r="W16" s="15"/>
+      <c r="W16" s="15">
+        <v>-23.818999999999999</v>
+      </c>
     </row>
     <row r="17" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -21896,65 +21958,65 @@
         <v>364.58400000000097</v>
       </c>
       <c r="G17" s="14">
-        <f>G19*G18</f>
-        <v>603.20000000000005</v>
+        <f>G15-SUM(G16:G16)</f>
+        <v>612.18299999999977</v>
       </c>
       <c r="H17" s="59"/>
       <c r="I17" s="59"/>
       <c r="L17" s="11">
-        <f t="shared" ref="L17:Y17" si="8">L15-SUM(L16:L16)</f>
+        <f t="shared" ref="L17:Y17" si="10">L15-SUM(L16:L16)</f>
         <v>186.84099999999989</v>
       </c>
       <c r="M17" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>139.45600000000005</v>
       </c>
       <c r="N17" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>210.011</v>
       </c>
       <c r="O17" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>108.20500000000001</v>
       </c>
       <c r="P17" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>100.83600000000004</v>
       </c>
       <c r="Q17" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>82.091000000000065</v>
       </c>
       <c r="R17" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>140.16199999999992</v>
       </c>
       <c r="S17" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>41.495000000000054</v>
       </c>
       <c r="T17" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>62.727000000000203</v>
       </c>
       <c r="U17" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>137.15700000000012</v>
       </c>
       <c r="V17" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>244.68400000000003</v>
       </c>
       <c r="W17" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
+        <v>167.61499999999987</v>
+      </c>
+      <c r="X17" s="11">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="X17" s="11">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="Y17" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21973,7 +22035,7 @@
         <v>160.07300000000001</v>
       </c>
       <c r="G18" s="15">
-        <v>160</v>
+        <v>156.77600000000001</v>
       </c>
       <c r="H18" s="41"/>
       <c r="I18" s="41"/>
@@ -22010,7 +22072,9 @@
       <c r="V18" s="10">
         <v>155.93299999999999</v>
       </c>
-      <c r="W18" s="15"/>
+      <c r="W18" s="15">
+        <v>154.452</v>
+      </c>
       <c r="X18" s="10"/>
       <c r="Y18" s="10"/>
     </row>
@@ -22035,56 +22099,58 @@
         <v>2.2776108400542312</v>
       </c>
       <c r="G19" s="55">
-        <v>3.77</v>
+        <f>G17/G18</f>
+        <v>3.9048259937745557</v>
       </c>
       <c r="H19" s="56"/>
       <c r="I19" s="57"/>
       <c r="L19" s="2">
-        <f t="shared" ref="L19:V19" si="9">L17/L18</f>
+        <f t="shared" ref="L19:V19" si="11">L17/L18</f>
         <v>1.109691635188748</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.82817761255188904</v>
       </c>
       <c r="N19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.2568735412053385</v>
       </c>
       <c r="O19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.65223812221967725</v>
       </c>
       <c r="P19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.6123185105569019</v>
       </c>
       <c r="Q19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.50305173237900347</v>
       </c>
       <c r="R19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.86925404976309151</v>
       </c>
       <c r="S19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.25922547837549154</v>
       </c>
       <c r="T19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.39485959246879432</v>
       </c>
       <c r="U19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.86857153713167623</v>
       </c>
       <c r="V19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.5691611140682218</v>
       </c>
       <c r="W19" s="49">
-        <v>0.62</v>
+        <f>W17/W18</f>
+        <v>1.0852238883277645</v>
       </c>
       <c r="X19" s="50"/>
       <c r="Y19" s="50"/>
@@ -22113,7 +22179,9 @@
       <c r="T20" s="51"/>
       <c r="U20" s="51"/>
       <c r="V20" s="51"/>
-      <c r="W20" s="49"/>
+      <c r="W20" s="151">
+        <v>0.62</v>
+      </c>
       <c r="X20" s="50">
         <v>0.75</v>
       </c>
@@ -22141,57 +22209,57 @@
       </c>
       <c r="G21" s="6">
         <f>1-G5/G3</f>
-        <v>1</v>
+        <v>0.41620628935850845</v>
       </c>
       <c r="H21" s="46"/>
       <c r="I21" s="46"/>
       <c r="L21" s="3">
-        <f t="shared" ref="L21:W21" si="10">1-L5/L3</f>
+        <f t="shared" ref="L21:W21" si="12">1-L5/L3</f>
         <v>0.43671240143347323</v>
       </c>
       <c r="M21" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.41798422527706813</v>
       </c>
       <c r="N21" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.40491382193091296</v>
       </c>
       <c r="O21" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.40398733652359275</v>
       </c>
       <c r="P21" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.39887831773525362</v>
       </c>
       <c r="Q21" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.38463346130513842</v>
       </c>
       <c r="R21" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.37832549166289342</v>
       </c>
       <c r="S21" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.36181889577606796</v>
       </c>
       <c r="T21" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.38869921877805935</v>
       </c>
       <c r="U21" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.41778775562720438</v>
       </c>
       <c r="V21" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.42153116793431644</v>
       </c>
-      <c r="W21" s="6" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+      <c r="W21" s="6">
+        <f t="shared" si="12"/>
+        <v>0.43444552426279326</v>
       </c>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
@@ -22216,7 +22284,7 @@
       </c>
       <c r="G22" s="7">
         <f>G17/G3</f>
-        <v>0.14226415094339623</v>
+        <v>0.14241891353359229</v>
       </c>
       <c r="H22" s="47">
         <f>H17/H4</f>
@@ -22227,52 +22295,52 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L22" s="4">
-        <f t="shared" ref="L22:W22" si="11">L17/L3</f>
+        <f t="shared" ref="L22:W22" si="13">L17/L3</f>
         <v>0.14240300352575869</v>
       </c>
       <c r="M22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.10675918476084907</v>
       </c>
       <c r="N22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.12862157961075024</v>
       </c>
       <c r="O22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.7971973847026916E-2</v>
       </c>
       <c r="P22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.6937703956926057E-2</v>
       </c>
       <c r="Q22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7.1448651857215897E-2</v>
       </c>
       <c r="R22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.11037029745851128</v>
       </c>
       <c r="S22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4.3220491689729107E-2</v>
       </c>
       <c r="T22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6.4368460101036737E-2</v>
       </c>
       <c r="U22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.12975966123246005</v>
       </c>
       <c r="V22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.19489387665047359</v>
       </c>
-      <c r="W22" s="7" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+      <c r="W22" s="7">
+        <f t="shared" si="13"/>
+        <v>0.16571147231748887</v>
       </c>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.25">
@@ -22294,11 +22362,11 @@
       </c>
       <c r="G23" s="6">
         <f>G3/F3-1</f>
-        <v>-6.5836083315083394E-2</v>
+        <v>-5.2954535740362463E-2</v>
       </c>
       <c r="H23" s="48">
         <f>H4/G3-1</f>
-        <v>3.7735849056603765E-2</v>
+        <v>2.3620746652236901E-2</v>
       </c>
       <c r="I23" s="48">
         <f>I4/H4-1</f>
@@ -22309,36 +22377,36 @@
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4">
-        <f t="shared" ref="P23:W23" si="12">P3/L3-1</f>
+        <f t="shared" ref="P23:W23" si="14">P3/L3-1</f>
         <v>-0.11599563433933557</v>
       </c>
       <c r="Q23" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-0.12043173409417829</v>
       </c>
       <c r="R23" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-0.22223236169923477</v>
       </c>
       <c r="S23" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-0.21944578591440278</v>
       </c>
       <c r="T23" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-0.15981687523979082</v>
       </c>
       <c r="U23" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-8.0023430067948875E-2</v>
       </c>
       <c r="V23" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-1.1380199618087672E-2</v>
       </c>
       <c r="W23" s="7">
-        <f t="shared" si="12"/>
-        <v>-1</v>
+        <f t="shared" si="14"/>
+        <v>5.3547788354475712E-2</v>
       </c>
       <c r="X23" s="37">
         <f>X4/T3-1</f>
@@ -22354,74 +22422,74 @@
         <v>63</v>
       </c>
       <c r="C24" s="4" t="e">
-        <f t="shared" ref="C24:G24" si="13">C7/C3</f>
+        <f t="shared" ref="C24:G24" si="15">C7/C3</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D24" s="4" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.18717024189118212</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.17828033642239013</v>
       </c>
       <c r="G24" s="7">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>0.16990010624718069</v>
       </c>
       <c r="H24" s="123"/>
       <c r="I24" s="123"/>
       <c r="L24" s="4">
-        <f t="shared" ref="L24:U24" si="14">L7/L3</f>
+        <f t="shared" ref="L24:U24" si="16">L7/L3</f>
         <v>0.19230399875615253</v>
       </c>
       <c r="M24" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.19645830446608542</v>
       </c>
       <c r="N24" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.16532580589447948</v>
       </c>
       <c r="O24" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.20082780891614108</v>
       </c>
       <c r="P24" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.19776267065563663</v>
       </c>
       <c r="Q24" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.17589174821206474</v>
       </c>
       <c r="R24" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.15485402681260704</v>
       </c>
       <c r="S24" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.18858904025406295</v>
       </c>
       <c r="T24" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.18387397011182155</v>
       </c>
       <c r="U24" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.16684452719373929</v>
       </c>
       <c r="V24" s="4">
         <f>V7/V3</f>
         <v>0.15068026154286077</v>
       </c>
-      <c r="W24" s="7" t="e">
+      <c r="W24" s="7">
         <f>W7/W3</f>
-        <v>#DIV/0!</v>
+        <v>0.1834862929528506</v>
       </c>
       <c r="X24" s="4"/>
     </row>
@@ -22430,74 +22498,74 @@
         <v>128</v>
       </c>
       <c r="C25" s="4" t="e">
-        <f t="shared" ref="C25:G25" si="15">C8/C3</f>
+        <f t="shared" ref="C25:G25" si="17">C8/C3</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D25" s="4" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5.324550669655604E-2</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6.1865446025815528E-2</v>
       </c>
       <c r="G25" s="7">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>6.6824521393324648E-2</v>
       </c>
       <c r="H25" s="123"/>
       <c r="I25" s="123"/>
       <c r="L25" s="4">
-        <f t="shared" ref="L25:U25" si="16">L8/L3</f>
+        <f t="shared" ref="L25:U25" si="18">L8/L3</f>
         <v>5.2776630301404358E-2</v>
       </c>
       <c r="M25" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.2562760905695387E-2</v>
       </c>
       <c r="N25" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>4.6257859285562926E-2</v>
       </c>
       <c r="O25" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>6.3746652422694755E-2</v>
       </c>
       <c r="P25" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>6.510843934423402E-2</v>
       </c>
       <c r="Q25" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>6.0062613636264729E-2</v>
       </c>
       <c r="R25" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.1688091816445854E-2</v>
       </c>
       <c r="S25" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>7.3567015978926689E-2</v>
       </c>
       <c r="T25" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>7.2405410369841314E-2</v>
       </c>
       <c r="U25" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>6.4861382316879337E-2</v>
       </c>
       <c r="V25" s="4">
         <f>V8/V3</f>
         <v>5.7909648395465294E-2</v>
       </c>
-      <c r="W25" s="7" t="e">
+      <c r="W25" s="7">
         <f>W8/W3</f>
-        <v>#DIV/0!</v>
+        <v>7.4564477843017271E-2</v>
       </c>
       <c r="X25" s="4"/>
     </row>
@@ -22506,74 +22574,74 @@
         <v>129</v>
       </c>
       <c r="C26" s="4" t="e">
-        <f t="shared" ref="C26:G26" si="17">C9/C3</f>
+        <f t="shared" ref="C26:G26" si="19">C9/C3</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D26" s="4" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.7120098680903711E-2</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.7463537863822694E-2</v>
       </c>
       <c r="G26" s="7">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>3.607239511202482E-2</v>
       </c>
       <c r="H26" s="123"/>
       <c r="I26" s="123"/>
       <c r="L26" s="4">
-        <f t="shared" ref="L26:U26" si="18">L9/L3</f>
+        <f t="shared" ref="L26:U26" si="20">L9/L3</f>
         <v>3.0899548648001842E-2</v>
       </c>
       <c r="M26" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>2.5470290530190228E-2</v>
       </c>
       <c r="N26" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>2.3565913881951176E-2</v>
       </c>
       <c r="O26" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>2.9558680774052559E-2</v>
       </c>
       <c r="P26" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.0917391248119392E-2</v>
       </c>
       <c r="Q26" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>2.3141979074825642E-2</v>
       </c>
       <c r="R26" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>2.3439179479103095E-2</v>
       </c>
       <c r="S26" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.3785831761410798E-2</v>
       </c>
       <c r="T26" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>4.2377673040198086E-2</v>
       </c>
       <c r="U26" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.3621316016529672E-2</v>
       </c>
       <c r="V26" s="4">
         <f>V9/V3</f>
         <v>3.1630309851346863E-2</v>
       </c>
-      <c r="W26" s="7" t="e">
+      <c r="W26" s="7">
         <f>W9/W3</f>
-        <v>#DIV/0!</v>
+        <v>3.807265936190974E-2</v>
       </c>
       <c r="X26" s="4"/>
     </row>
@@ -22596,11 +22664,11 @@
       </c>
       <c r="G27" s="6">
         <f>G17/F17-1</f>
-        <v>0.65448840322120128</v>
+        <v>0.67912744388124047</v>
       </c>
       <c r="H27" s="58">
         <f>H20/G19-1</f>
-        <v>4.5092838196286511E-2</v>
+        <v>9.0078293582152025E-3</v>
       </c>
       <c r="I27" s="58" t="e">
         <f>I19/H19-1</f>
@@ -22611,39 +22679,39 @@
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4">
-        <f t="shared" ref="P27:X27" si="19">P17/L17-1</f>
+        <f t="shared" ref="P27:X27" si="21">P17/L17-1</f>
         <v>-0.46031117367173102</v>
       </c>
       <c r="Q27" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>-0.41134838228545179</v>
       </c>
       <c r="R27" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>-0.33259686397379218</v>
       </c>
       <c r="S27" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>-0.61651494847742661</v>
       </c>
       <c r="T27" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>-0.37793050101154169</v>
       </c>
       <c r="U27" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.67079216966537158</v>
       </c>
       <c r="V27" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.74572280646680378</v>
       </c>
       <c r="W27" s="7">
-        <f t="shared" si="19"/>
-        <v>-1</v>
+        <f t="shared" si="21"/>
+        <v>3.0394023376310315</v>
       </c>
       <c r="X27" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>-1</v>
       </c>
     </row>
@@ -22652,72 +22720,72 @@
         <v>36</v>
       </c>
       <c r="C30" s="11">
-        <f t="shared" ref="C30:F30" si="20">C31</f>
+        <f t="shared" ref="C30:F30" si="22">C31</f>
         <v>0</v>
       </c>
       <c r="D30" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="E30" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1328.7159999999999</v>
       </c>
       <c r="F30" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1149.0229999999999</v>
       </c>
       <c r="G30" s="14">
         <f>G31</f>
+        <v>1520.8420000000001</v>
+      </c>
+      <c r="L30" s="11">
+        <f t="shared" ref="L30" si="23">L31</f>
         <v>0</v>
       </c>
-      <c r="L30" s="11">
-        <f t="shared" ref="L30" si="21">L31</f>
+      <c r="M30" s="11">
+        <f t="shared" ref="M30" si="24">M31</f>
         <v>0</v>
       </c>
-      <c r="M30" s="11">
-        <f t="shared" ref="M30" si="22">M31</f>
+      <c r="N30" s="11">
+        <f t="shared" ref="N30" si="25">N31</f>
         <v>0</v>
       </c>
-      <c r="N30" s="11">
-        <f t="shared" ref="N30" si="23">N31</f>
-        <v>0</v>
-      </c>
       <c r="O30" s="11">
-        <f t="shared" ref="O30" si="24">O31</f>
+        <f t="shared" ref="O30" si="26">O31</f>
         <v>1328.7159999999999</v>
       </c>
       <c r="P30" s="11">
-        <f t="shared" ref="P30" si="25">P31</f>
+        <f t="shared" ref="P30" si="27">P31</f>
         <v>1106.6569999999999</v>
       </c>
       <c r="Q30" s="11">
-        <f t="shared" ref="Q30" si="26">Q31</f>
+        <f t="shared" ref="Q30" si="28">Q31</f>
         <v>868.50099999999998</v>
       </c>
       <c r="R30" s="11">
-        <f t="shared" ref="R30" si="27">R31</f>
+        <f t="shared" ref="R30" si="29">R31</f>
         <v>1036.1310000000001</v>
       </c>
       <c r="S30" s="11">
-        <f t="shared" ref="S30" si="28">S31</f>
+        <f t="shared" ref="S30" si="30">S31</f>
         <v>1149.0229999999999</v>
       </c>
       <c r="T30" s="11">
-        <f t="shared" ref="T30" si="29">T31</f>
+        <f t="shared" ref="T30" si="31">T31</f>
         <v>1251.086</v>
       </c>
       <c r="U30" s="11">
-        <f t="shared" ref="U30" si="30">U31</f>
+        <f t="shared" ref="U30" si="32">U31</f>
         <v>1163.904</v>
       </c>
       <c r="V30" s="11">
-        <f t="shared" ref="V30" si="31">V31</f>
+        <f t="shared" ref="V30" si="33">V31</f>
         <v>1412.65</v>
       </c>
       <c r="W30" s="14">
-        <f t="shared" ref="W30" si="32">W31</f>
-        <v>0</v>
+        <f>W31</f>
+        <v>1520.8420000000001</v>
       </c>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.25">
@@ -22732,7 +22800,10 @@
       <c r="F31" s="10">
         <v>1149.0229999999999</v>
       </c>
-      <c r="G31" s="15"/>
+      <c r="G31" s="15">
+        <f>W31</f>
+        <v>1520.8420000000001</v>
+      </c>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
@@ -22762,7 +22833,9 @@
       <c r="V31" s="10">
         <v>1412.65</v>
       </c>
-      <c r="W31" s="15"/>
+      <c r="W31" s="15">
+        <v>1520.8420000000001</v>
+      </c>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
@@ -22776,12 +22849,15 @@
       <c r="F32" s="10">
         <v>630.38199999999995</v>
       </c>
-      <c r="G32" s="15"/>
+      <c r="G32" s="15">
+        <f t="shared" ref="G32:G34" si="34">W32</f>
+        <v>541.71500000000003</v>
+      </c>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
       <c r="O32" s="10">
-        <f t="shared" ref="O32:O34" si="33">E32</f>
+        <f t="shared" ref="O32:O34" si="35">E32</f>
         <v>675.60400000000004</v>
       </c>
       <c r="P32" s="10">
@@ -22794,7 +22870,7 @@
         <v>802.43499999999995</v>
       </c>
       <c r="S32" s="10">
-        <f t="shared" ref="S32:S34" si="34">F32</f>
+        <f t="shared" ref="S32:S34" si="36">F32</f>
         <v>630.38199999999995</v>
       </c>
       <c r="T32" s="10">
@@ -22806,7 +22882,9 @@
       <c r="V32" s="10">
         <v>685.77700000000004</v>
       </c>
-      <c r="W32" s="15"/>
+      <c r="W32" s="15">
+        <v>541.71500000000003</v>
+      </c>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
@@ -22820,12 +22898,15 @@
       <c r="F33" s="10">
         <v>682.89300000000003</v>
       </c>
-      <c r="G33" s="15"/>
+      <c r="G33" s="15">
+        <f t="shared" si="34"/>
+        <v>422.51299999999998</v>
+      </c>
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
       <c r="O33" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>933.12400000000002</v>
       </c>
       <c r="P33" s="10">
@@ -22838,7 +22919,7 @@
         <v>797.69500000000005</v>
       </c>
       <c r="S33" s="10">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>682.89300000000003</v>
       </c>
       <c r="T33" s="10">
@@ -22850,7 +22931,9 @@
       <c r="V33" s="10">
         <v>447.262</v>
       </c>
-      <c r="W33" s="15"/>
+      <c r="W33" s="15">
+        <v>422.51299999999998</v>
+      </c>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
@@ -22864,12 +22947,15 @@
       <c r="F34" s="10">
         <v>142.876</v>
       </c>
-      <c r="G34" s="15"/>
+      <c r="G34" s="15">
+        <f t="shared" si="34"/>
+        <v>146.27000000000001</v>
+      </c>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>135.47800000000001</v>
       </c>
       <c r="P34" s="10">
@@ -22882,7 +22968,7 @@
         <v>125.08799999999999</v>
       </c>
       <c r="S34" s="10">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>142.876</v>
       </c>
       <c r="T34" s="10">
@@ -22894,7 +22980,9 @@
       <c r="V34" s="10">
         <v>150.75399999999999</v>
       </c>
-      <c r="W34" s="15"/>
+      <c r="W34" s="15">
+        <v>146.27000000000001</v>
+      </c>
     </row>
     <row r="35" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
@@ -22918,55 +23006,55 @@
       </c>
       <c r="G35" s="14">
         <f>SUM(G31:G34)</f>
+        <v>2631.34</v>
+      </c>
+      <c r="L35" s="11">
+        <f t="shared" ref="L35:W35" si="37">SUM(L31:L34)</f>
         <v>0</v>
       </c>
-      <c r="L35" s="11">
-        <f t="shared" ref="L35:W35" si="35">SUM(L31:L34)</f>
+      <c r="M35" s="11">
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="M35" s="11">
-        <f t="shared" si="35"/>
+      <c r="N35" s="11">
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="N35" s="11">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
       <c r="O35" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>3072.922</v>
       </c>
       <c r="P35" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>2857.5879999999997</v>
       </c>
       <c r="Q35" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>2658.1350000000002</v>
       </c>
       <c r="R35" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>2761.3490000000002</v>
       </c>
       <c r="S35" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>2605.174</v>
       </c>
       <c r="T35" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>2497.6040000000003</v>
       </c>
       <c r="U35" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>2492.2240000000002</v>
       </c>
       <c r="V35" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>2696.4430000000002</v>
       </c>
       <c r="W35" s="14">
-        <f t="shared" si="35"/>
-        <v>0</v>
+        <f t="shared" si="37"/>
+        <v>2631.34</v>
       </c>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.25">
@@ -22981,12 +23069,15 @@
       <c r="F36" s="10">
         <v>121.503</v>
       </c>
-      <c r="G36" s="15"/>
+      <c r="G36" s="15">
+        <f t="shared" ref="G36:G39" si="38">W36</f>
+        <v>116.589</v>
+      </c>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
       <c r="O36" s="10">
-        <f t="shared" ref="O36:O39" si="36">E36</f>
+        <f t="shared" ref="O36:O39" si="39">E36</f>
         <v>109.807</v>
       </c>
       <c r="P36" s="10">
@@ -22999,7 +23090,7 @@
         <v>118.18300000000001</v>
       </c>
       <c r="S36" s="10">
-        <f t="shared" ref="S36:S39" si="37">F36</f>
+        <f t="shared" ref="S36:S39" si="40">F36</f>
         <v>121.503</v>
       </c>
       <c r="T36" s="10">
@@ -23011,7 +23102,9 @@
       <c r="V36" s="10">
         <v>119.2</v>
       </c>
-      <c r="W36" s="15"/>
+      <c r="W36" s="15">
+        <v>116.589</v>
+      </c>
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -23025,12 +23118,15 @@
       <c r="F37" s="10">
         <v>454.61</v>
       </c>
-      <c r="G37" s="15"/>
+      <c r="G37" s="15">
+        <f t="shared" si="38"/>
+        <v>461.97800000000001</v>
+      </c>
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
       <c r="O37" s="10">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>448.17500000000001</v>
       </c>
       <c r="P37" s="10">
@@ -23043,7 +23139,7 @@
         <v>454.471</v>
       </c>
       <c r="S37" s="10">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>454.61</v>
       </c>
       <c r="T37" s="10">
@@ -23055,7 +23151,9 @@
       <c r="V37" s="10">
         <v>463.97800000000001</v>
       </c>
-      <c r="W37" s="15"/>
+      <c r="W37" s="15">
+        <v>461.97800000000001</v>
+      </c>
     </row>
     <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -23069,12 +23167,15 @@
       <c r="F38" s="10">
         <v>63.173000000000002</v>
       </c>
-      <c r="G38" s="15"/>
+      <c r="G38" s="15">
+        <f t="shared" si="38"/>
+        <v>44.603000000000002</v>
+      </c>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
       <c r="O38" s="10">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>83.778999999999996</v>
       </c>
       <c r="P38" s="10">
@@ -23087,7 +23188,7 @@
         <v>69.364000000000004</v>
       </c>
       <c r="S38" s="10">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>63.173000000000002</v>
       </c>
       <c r="T38" s="10">
@@ -23099,7 +23200,9 @@
       <c r="V38" s="10">
         <v>53.723999999999997</v>
       </c>
-      <c r="W38" s="15"/>
+      <c r="W38" s="15">
+        <v>44.603000000000002</v>
+      </c>
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -23113,12 +23216,15 @@
       <c r="F39" s="10">
         <v>316.29300000000001</v>
       </c>
-      <c r="G39" s="15"/>
+      <c r="G39" s="15">
+        <f t="shared" si="38"/>
+        <v>350.19400000000002</v>
+      </c>
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
       <c r="O39" s="10">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>320.72199999999998</v>
       </c>
       <c r="P39" s="10">
@@ -23131,7 +23237,7 @@
         <v>335.87900000000002</v>
       </c>
       <c r="S39" s="10">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>316.29300000000001</v>
       </c>
       <c r="T39" s="10">
@@ -23143,7 +23249,9 @@
       <c r="V39" s="10">
         <v>326.59399999999999</v>
       </c>
-      <c r="W39" s="15"/>
+      <c r="W39" s="15">
+        <v>350.19400000000002</v>
+      </c>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
@@ -23167,55 +23275,55 @@
       </c>
       <c r="G40" s="14">
         <f>SUM(G35:G39)</f>
+        <v>3604.7040000000002</v>
+      </c>
+      <c r="L40" s="11">
+        <f t="shared" ref="L40:W40" si="41">SUM(L35:L39)</f>
         <v>0</v>
       </c>
-      <c r="L40" s="11">
-        <f t="shared" ref="L40:W40" si="38">SUM(L35:L39)</f>
+      <c r="M40" s="11">
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="M40" s="11">
-        <f t="shared" si="38"/>
+      <c r="N40" s="11">
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="N40" s="11">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
       <c r="O40" s="11">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>4035.4049999999997</v>
       </c>
       <c r="P40" s="11">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>3829.7119999999995</v>
       </c>
       <c r="Q40" s="11">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>3644.8990000000003</v>
       </c>
       <c r="R40" s="11">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>3739.2460000000001</v>
       </c>
       <c r="S40" s="11">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>3560.7530000000002</v>
       </c>
       <c r="T40" s="11">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>3439.8810000000003</v>
       </c>
       <c r="U40" s="11">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>3425.03</v>
       </c>
       <c r="V40" s="11">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>3659.9390000000003</v>
       </c>
       <c r="W40" s="14">
-        <f t="shared" si="38"/>
-        <v>0</v>
+        <f t="shared" si="41"/>
+        <v>3604.7040000000002</v>
       </c>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.25">
@@ -23230,12 +23338,15 @@
       <c r="F41" s="10">
         <v>406.96800000000002</v>
       </c>
-      <c r="G41" s="15"/>
+      <c r="G41" s="15">
+        <f t="shared" ref="G41:G42" si="42">W41</f>
+        <v>448.62700000000001</v>
+      </c>
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
       <c r="O41" s="10">
-        <f t="shared" ref="O41:O42" si="39">E41</f>
+        <f t="shared" ref="O41:O42" si="43">E41</f>
         <v>636.30600000000004</v>
       </c>
       <c r="P41" s="10">
@@ -23248,7 +23359,7 @@
         <v>491.488</v>
       </c>
       <c r="S41" s="10">
-        <f t="shared" ref="S41:S42" si="40">F41</f>
+        <f t="shared" ref="S41:S42" si="44">F41</f>
         <v>406.96800000000002</v>
       </c>
       <c r="T41" s="10">
@@ -23260,7 +23371,9 @@
       <c r="V41" s="10">
         <v>527.98800000000006</v>
       </c>
-      <c r="W41" s="15"/>
+      <c r="W41" s="15">
+        <v>448.62700000000001</v>
+      </c>
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
@@ -23274,12 +23387,15 @@
       <c r="F42" s="10">
         <v>643.13900000000001</v>
       </c>
-      <c r="G42" s="15"/>
+      <c r="G42" s="15">
+        <f t="shared" si="42"/>
+        <v>637.26199999999994</v>
+      </c>
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
       <c r="O42" s="10">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>784.84799999999996</v>
       </c>
       <c r="P42" s="10">
@@ -23292,7 +23408,7 @@
         <v>705.56899999999996</v>
       </c>
       <c r="S42" s="10">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>643.13900000000001</v>
       </c>
       <c r="T42" s="10">
@@ -23304,7 +23420,9 @@
       <c r="V42" s="10">
         <v>673.43499999999995</v>
       </c>
-      <c r="W42" s="15"/>
+      <c r="W42" s="15">
+        <v>637.26199999999994</v>
+      </c>
     </row>
     <row r="43" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
@@ -23328,55 +23446,55 @@
       </c>
       <c r="G43" s="14">
         <f>SUM(G41:G42)</f>
+        <v>1085.8889999999999</v>
+      </c>
+      <c r="L43" s="11">
+        <f t="shared" ref="L43:W43" si="45">SUM(L41:L42)</f>
         <v>0</v>
       </c>
-      <c r="L43" s="11">
-        <f t="shared" ref="L43:W43" si="41">SUM(L41:L42)</f>
+      <c r="M43" s="11">
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="M43" s="11">
-        <f t="shared" si="41"/>
+      <c r="N43" s="11">
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="N43" s="11">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
       <c r="O43" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>1421.154</v>
       </c>
       <c r="P43" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>1252.7669999999998</v>
       </c>
       <c r="Q43" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>1210.184</v>
       </c>
       <c r="R43" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>1197.057</v>
       </c>
       <c r="S43" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>1050.107</v>
       </c>
       <c r="T43" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>957.14300000000003</v>
       </c>
       <c r="U43" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>1086.9470000000001</v>
       </c>
       <c r="V43" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>1201.423</v>
       </c>
       <c r="W43" s="14">
-        <f t="shared" si="41"/>
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>1085.8889999999999</v>
       </c>
       <c r="X43" s="11"/>
       <c r="Y43" s="11"/>
@@ -23393,12 +23511,15 @@
       <c r="F44" s="10">
         <v>106.39100000000001</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="15">
+        <f t="shared" ref="G44:G45" si="46">W44</f>
+        <v>112.572</v>
+      </c>
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
       <c r="O44" s="10">
-        <f t="shared" ref="O44:O45" si="42">E44</f>
+        <f t="shared" ref="O44:O45" si="47">E44</f>
         <v>83.38</v>
       </c>
       <c r="P44" s="10">
@@ -23411,7 +23532,7 @@
         <v>117.608</v>
       </c>
       <c r="S44" s="10">
-        <f t="shared" ref="S44:S45" si="43">F44</f>
+        <f t="shared" ref="S44:S45" si="48">F44</f>
         <v>106.39100000000001</v>
       </c>
       <c r="T44" s="10">
@@ -23423,7 +23544,9 @@
       <c r="V44" s="10">
         <v>111.92400000000001</v>
       </c>
-      <c r="W44" s="15"/>
+      <c r="W44" s="15">
+        <v>112.572</v>
+      </c>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -23437,12 +23560,15 @@
       <c r="F45" s="10">
         <v>146.69499999999999</v>
       </c>
-      <c r="G45" s="15"/>
+      <c r="G45" s="15">
+        <f t="shared" si="46"/>
+        <v>172.59</v>
+      </c>
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
       <c r="O45" s="10">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>132.13300000000001</v>
       </c>
       <c r="P45" s="10">
@@ -23455,7 +23581,7 @@
         <v>165.91499999999999</v>
       </c>
       <c r="S45" s="10">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>146.69499999999999</v>
       </c>
       <c r="T45" s="10">
@@ -23467,7 +23593,9 @@
       <c r="V45" s="10">
         <v>156.49100000000001</v>
       </c>
-      <c r="W45" s="15"/>
+      <c r="W45" s="15">
+        <v>172.59</v>
+      </c>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
@@ -23491,55 +23619,55 @@
       </c>
       <c r="G46" s="14">
         <f>SUM(G43:G45)</f>
+        <v>1371.0509999999997</v>
+      </c>
+      <c r="L46" s="11">
+        <f t="shared" ref="L46:W46" si="49">SUM(L43:L45)</f>
         <v>0</v>
       </c>
-      <c r="L46" s="11">
-        <f t="shared" ref="L46:W46" si="44">SUM(L43:L45)</f>
+      <c r="M46" s="11">
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
-      <c r="M46" s="11">
-        <f t="shared" si="44"/>
+      <c r="N46" s="11">
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
-      <c r="N46" s="11">
-        <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
       <c r="O46" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>1636.6670000000001</v>
       </c>
       <c r="P46" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>1467.3539999999998</v>
       </c>
       <c r="Q46" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>1476.338</v>
       </c>
       <c r="R46" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>1480.58</v>
       </c>
       <c r="S46" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>1303.193</v>
       </c>
       <c r="T46" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>1213.806</v>
       </c>
       <c r="U46" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>1347.7650000000001</v>
       </c>
       <c r="V46" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>1469.838</v>
       </c>
       <c r="W46" s="14">
-        <f t="shared" si="44"/>
-        <v>0</v>
+        <f t="shared" si="49"/>
+        <v>1371.0509999999997</v>
       </c>
     </row>
     <row r="47" spans="2:25" x14ac:dyDescent="0.25">
@@ -23564,26 +23692,26 @@
       </c>
       <c r="G47" s="15">
         <f>G40-G46</f>
+        <v>2233.6530000000002</v>
+      </c>
+      <c r="N47" s="10">
+        <f t="shared" ref="N47:R47" si="50">N40-N46</f>
         <v>0</v>
       </c>
-      <c r="N47" s="10">
-        <f t="shared" ref="N47:R47" si="45">N40-N46</f>
-        <v>0</v>
-      </c>
       <c r="O47" s="10">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>2398.7379999999994</v>
       </c>
       <c r="P47" s="10">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>2362.3579999999997</v>
       </c>
       <c r="Q47" s="10">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>2168.5610000000006</v>
       </c>
       <c r="R47" s="10">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>2258.6660000000002</v>
       </c>
       <c r="S47" s="10">
@@ -23591,20 +23719,20 @@
         <v>2257.5600000000004</v>
       </c>
       <c r="T47" s="10">
-        <f t="shared" ref="T47:W47" si="46">T40-T46</f>
+        <f t="shared" ref="T47:W47" si="51">T40-T46</f>
         <v>2226.0750000000003</v>
       </c>
       <c r="U47" s="10">
-        <f t="shared" si="46"/>
+        <f t="shared" si="51"/>
         <v>2077.2650000000003</v>
       </c>
       <c r="V47" s="10">
-        <f t="shared" si="46"/>
+        <f t="shared" si="51"/>
         <v>2190.1010000000006</v>
       </c>
       <c r="W47" s="15">
-        <f t="shared" si="46"/>
-        <v>0</v>
+        <f t="shared" si="51"/>
+        <v>2233.6530000000002</v>
       </c>
     </row>
     <row r="49" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -23669,10 +23797,10 @@
   <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O27" sqref="O27"/>
+      <selection pane="bottomRight" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23830,7 +23958,9 @@
       <c r="S3" s="10">
         <v>409.04300000000001</v>
       </c>
-      <c r="T3" s="10"/>
+      <c r="T3" s="10">
+        <v>273</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -23877,7 +24007,9 @@
       <c r="S4" s="10">
         <v>229.43199999999999</v>
       </c>
-      <c r="T4" s="10"/>
+      <c r="T4" s="10">
+        <v>216</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -23924,7 +24056,9 @@
       <c r="S5" s="10">
         <v>206.18</v>
       </c>
-      <c r="T5" s="10"/>
+      <c r="T5" s="10">
+        <v>171</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -23971,7 +24105,9 @@
       <c r="S6" s="10">
         <v>169.52199999999999</v>
       </c>
-      <c r="T6" s="10"/>
+      <c r="T6" s="10">
+        <v>148</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -24018,7 +24154,9 @@
       <c r="S7" s="10">
         <v>85.850999999999999</v>
       </c>
-      <c r="T7" s="10"/>
+      <c r="T7" s="10">
+        <v>76</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -24065,7 +24203,9 @@
       <c r="S8" s="10">
         <v>64.239000000000004</v>
       </c>
-      <c r="T8" s="10"/>
+      <c r="T8" s="10">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -24112,7 +24252,9 @@
       <c r="S9" s="10">
         <v>41.762</v>
       </c>
-      <c r="T9" s="10"/>
+      <c r="T9" s="10">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -24163,7 +24305,9 @@
       <c r="S10" s="10">
         <v>49.444000000000003</v>
       </c>
-      <c r="T10" s="10"/>
+      <c r="T10" s="10">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -24234,7 +24378,7 @@
       </c>
       <c r="T11" s="10">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -24245,7 +24389,7 @@
       <c r="L13" s="127"/>
       <c r="M13" s="127"/>
       <c r="N13" s="128">
-        <f t="shared" ref="N13:S15" si="11">N3/J3-1</f>
+        <f t="shared" ref="N13:T15" si="11">N3/J3-1</f>
         <v>-2.7190332326283984E-2</v>
       </c>
       <c r="O13" s="128">
@@ -24268,6 +24412,10 @@
         <f t="shared" si="11"/>
         <v>-7.0012405110614351E-3</v>
       </c>
+      <c r="T13" s="149">
+        <f>T3/P3-1</f>
+        <v>0.14212560871529689</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -24297,6 +24445,10 @@
         <f t="shared" si="11"/>
         <v>4.2593122753443291E-2</v>
       </c>
+      <c r="T14" s="149">
+        <f t="shared" si="11"/>
+        <v>0.15015974440894553</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -24318,13 +24470,17 @@
         <f t="shared" si="11"/>
         <v>-4.8171407059028781E-2</v>
       </c>
-      <c r="R15" s="127">
+      <c r="R15" s="150">
         <f t="shared" si="11"/>
         <v>3.7837837837837895E-2</v>
       </c>
-      <c r="S15" s="127">
+      <c r="S15" s="150">
         <f t="shared" si="11"/>
         <v>3.5528813797675696E-2</v>
+      </c>
+      <c r="T15" s="150">
+        <f t="shared" si="11"/>
+        <v>6.3644506369426646E-2</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -24336,7 +24492,7 @@
         <v>-0.22844827586206895</v>
       </c>
       <c r="O16" s="128">
-        <f t="shared" ref="O16:S16" si="12">O6/K6-1</f>
+        <f t="shared" ref="O16:T16" si="12">O6/K6-1</f>
         <v>-0.39541463414634148</v>
       </c>
       <c r="P16" s="128">
@@ -24355,8 +24511,12 @@
         <f t="shared" si="12"/>
         <v>-2.301805020862624E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="128">
+        <f>T6/P6-1</f>
+        <v>-0.17189362190229462</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>199</v>
       </c>
@@ -24390,8 +24550,11 @@
       <c r="S19">
         <v>539</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>200</v>
       </c>
@@ -24425,8 +24588,11 @@
       <c r="S20">
         <v>300</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>201</v>
       </c>
@@ -24460,13 +24626,16 @@
       <c r="S21">
         <v>417</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>202</v>
       </c>
       <c r="N23" s="128">
-        <f t="shared" ref="N23:S23" si="13">N19/J19-1</f>
+        <f t="shared" ref="N23:T23" si="13">N19/J19-1</f>
         <v>-9.2250922509225064E-2</v>
       </c>
       <c r="O23" s="128">
@@ -24485,12 +24654,16 @@
         <f t="shared" si="13"/>
         <v>-6.0975609756097615E-2</v>
       </c>
-      <c r="S23" s="127">
+      <c r="S23" s="150">
         <f t="shared" si="13"/>
         <v>4.8638132295719894E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23" s="150">
+        <f t="shared" si="13"/>
+        <v>6.3829787234042534E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>203</v>
       </c>
@@ -24503,7 +24676,7 @@
         <v>-0.40579710144927539</v>
       </c>
       <c r="P24" s="128">
-        <f t="shared" ref="N24:S25" si="14">P20/L20-1</f>
+        <f t="shared" ref="N24:T25" si="14">P20/L20-1</f>
         <v>-0.31642512077294682</v>
       </c>
       <c r="Q24" s="128">
@@ -24518,8 +24691,12 @@
         <f t="shared" si="14"/>
         <v>-8.536585365853655E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24" s="150">
+        <f t="shared" si="14"/>
+        <v>0.10954063604240272</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>204</v>
       </c>
@@ -24546,6 +24723,10 @@
       <c r="S25" s="128">
         <f t="shared" si="14"/>
         <v>-2.7972027972028024E-2</v>
+      </c>
+      <c r="T25" s="128">
+        <f t="shared" si="14"/>
+        <v>-2.7559055118110187E-2</v>
       </c>
     </row>
   </sheetData>
@@ -38545,7 +38726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366AC5E7-7FF6-4287-9F23-7D3A6FE15A5F}">
   <dimension ref="A1:M1415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>

</xml_diff>